<commit_message>
Sum instead of mean fix
</commit_message>
<xml_diff>
--- a/excel/evaluation_GRI_template.xlsx
+++ b/excel/evaluation_GRI_template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sergio\SemanticsAI-Project\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DA75FCA-22B5-49DC-BDEE-730985544B4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A3991A3-5249-44B0-B74D-6BE2C3C79FA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1006,7 +1006,7 @@
     <t>SPECIFIC GRI ONLY</t>
   </si>
   <si>
-    <t>MEAN</t>
+    <t>TOTAL</t>
   </si>
 </sst>
 </file>
@@ -1674,9 +1674,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:EX404"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="EA1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A361" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="EN403" sqref="EN403"/>
+    <sheetView tabSelected="1" topLeftCell="EB1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A347" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="EI373" sqref="EI373"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -60964,55 +60964,55 @@
       <c r="DX403" s="34" t="s">
         <v>266</v>
       </c>
-      <c r="DY403" s="35" t="e">
-        <f>AVERAGE(DY2:DY402)</f>
+      <c r="DY403" s="35">
+        <f>SUM(DY2:DY402)</f>
+        <v>0</v>
+      </c>
+      <c r="DZ403" s="35">
+        <f>SUM(DZ2:DZ402)</f>
+        <v>0</v>
+      </c>
+      <c r="EA403" s="35">
+        <f>SUM(EA2:EA402)</f>
+        <v>0</v>
+      </c>
+      <c r="EB403" s="35">
+        <f>SUM(EB2:EB402)</f>
+        <v>0</v>
+      </c>
+      <c r="EC403" s="35" t="e">
+        <f t="shared" ref="DY403:ED403" si="0">AVERAGE(EC2:EC402)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="DZ403" s="35" t="e">
-        <f>AVERAGE(DZ2:DZ402)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="EA403" s="35" t="e">
-        <f>AVERAGE(EA2:EA402)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="EB403" s="35" t="e">
-        <f>AVERAGE(EB2:EB402)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="EC403" s="35" t="e">
-        <f>AVERAGE(EC2:EC402)</f>
-        <v>#DIV/0!</v>
-      </c>
       <c r="ED403" s="35" t="e">
-        <f>AVERAGE(ED2:ED402)</f>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="EG403" s="34" t="s">
         <v>266</v>
       </c>
-      <c r="EH403" s="35" t="e">
-        <f>AVERAGE(EH2:EH402)</f>
+      <c r="EH403" s="35">
+        <f>SUM(EH2:EH402)</f>
+        <v>0</v>
+      </c>
+      <c r="EI403" s="35">
+        <f>SUM(EI2:EI402)</f>
+        <v>0</v>
+      </c>
+      <c r="EJ403" s="35">
+        <f>SUM(EJ2:EJ402)</f>
+        <v>0</v>
+      </c>
+      <c r="EK403" s="35">
+        <f>SUM(EK2:EK402)</f>
+        <v>0</v>
+      </c>
+      <c r="EL403" s="35" t="e">
+        <f t="shared" ref="EH403:EM403" si="1">AVERAGE(EL2:EL402)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="EI403" s="35" t="e">
-        <f>AVERAGE(EI2:EI402)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="EJ403" s="35" t="e">
-        <f>AVERAGE(EJ2:EJ402)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="EK403" s="35" t="e">
-        <f>AVERAGE(EK2:EK402)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="EL403" s="35" t="e">
-        <f>AVERAGE(EL2:EL402)</f>
-        <v>#DIV/0!</v>
-      </c>
       <c r="EM403" s="35" t="e">
-        <f>AVERAGE(EM2:EM402)</f>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>

</xml_diff>